<commit_message>
course syllabus and structure changes
</commit_message>
<xml_diff>
--- a/Stat5100/course/S21 Schedule (Stat 5100).xlsx
+++ b/Stat5100/course/S21 Schedule (Stat 5100).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brennan\github\teaching\Stat5100\course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643E5937-7CA6-4E34-8F98-0EB695578E73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D93F78-BA59-45E3-B577-47F4757441FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -267,9 +267,6 @@
     <t xml:space="preserve">Model Interpretability </t>
   </si>
   <si>
-    <t xml:space="preserve">Mythos of Model Interpretability* </t>
-  </si>
-  <si>
     <t>* - Assignment due before class (1:15pm)</t>
   </si>
   <si>
@@ -277,6 +274,9 @@
   </si>
   <si>
     <t>HW 1/Getting to Know You/Hypothesis Testing Quiz/Syllabus Quiz</t>
+  </si>
+  <si>
+    <t>Mythos of Model Interpretability</t>
   </si>
 </sst>
 </file>
@@ -597,11 +597,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -885,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -898,11 +898,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
@@ -967,8 +967,8 @@
       <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="41" t="s">
-        <v>68</v>
+      <c r="C8" s="40" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1190,7 +1190,7 @@
         <v>40</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1209,7 +1209,7 @@
         <v>43916</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C32" s="22" t="s">
         <v>56</v>
@@ -1397,7 +1397,7 @@
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="13"/>
       <c r="B51" s="38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
changes up through module 3 based on ruth feedback
</commit_message>
<xml_diff>
--- a/Stat5100/course/S21 Schedule (Stat 5100).xlsx
+++ b/Stat5100/course/S21 Schedule (Stat 5100).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brennan\github\teaching\Stat5100\course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D93F78-BA59-45E3-B577-47F4757441FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080ECFC2-0752-4E04-86A0-223B2FE13344}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,9 +76,6 @@
     <t>2.4: Simultaneous Inference:</t>
   </si>
   <si>
-    <t>Intro to Scientific Writing</t>
-  </si>
-  <si>
     <t>4.1: Penalized Regression</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
     <t xml:space="preserve">Quiz 4 </t>
   </si>
   <si>
-    <t>Quiz 5</t>
-  </si>
-  <si>
     <t>Review Response/Final Project Papers - Final Draft</t>
   </si>
   <si>
@@ -163,9 +157,6 @@
     <t>4.3: Non-Parametric Regression</t>
   </si>
   <si>
-    <t xml:space="preserve">Final Project Papers - Penultimate Draft </t>
-  </si>
-  <si>
     <t>No Class (Interim Day)</t>
   </si>
   <si>
@@ -178,9 +169,6 @@
     <t>Final Project Proposals</t>
   </si>
   <si>
-    <t>Project 2 Peer Review</t>
-  </si>
-  <si>
     <t>HW 6</t>
   </si>
   <si>
@@ -221,9 +209,6 @@
   </si>
   <si>
     <t>Project 2 Papers - Final Draft</t>
-  </si>
-  <si>
-    <t>Final Project Update</t>
   </si>
   <si>
     <t>Quiz 6</t>
@@ -267,9 +252,6 @@
     <t xml:space="preserve">Model Interpretability </t>
   </si>
   <si>
-    <t>* - Assignment due before class (1:15pm)</t>
-  </si>
-  <si>
     <t>Group Work Primer</t>
   </si>
   <si>
@@ -277,6 +259,25 @@
   </si>
   <si>
     <t>Mythos of Model Interpretability</t>
+  </si>
+  <si>
+    <t>Regression in the real world</t>
+  </si>
+  <si>
+    <t>Intro to Scientific Writing/Writing Fellow Appointment</t>
+  </si>
+  <si>
+    <t>Project 2 Peer Review/Writing Fellow Appointment</t>
+  </si>
+  <si>
+    <t>Quiz 5/Final Project Update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(23-Apr) Final Project Papers - Penultimate Draft
+(24-Apr) Group Member Evaluation </t>
+  </si>
+  <si>
+    <t>* - Assignment due before class (1:00pm)</t>
   </si>
 </sst>
 </file>
@@ -585,7 +586,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -602,6 +602,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -885,24 +888,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.1796875" style="1" customWidth="1"/>
     <col min="2" max="2" width="48" customWidth="1"/>
-    <col min="3" max="3" width="45.54296875" customWidth="1"/>
+    <col min="3" max="3" width="48.26953125" customWidth="1"/>
     <col min="4" max="4" width="24.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
@@ -920,7 +923,7 @@
         <v>43848</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C3" s="18"/>
     </row>
@@ -929,7 +932,7 @@
         <v>43850</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C4" s="18"/>
     </row>
@@ -947,7 +950,7 @@
         <v>43855</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C6" s="21"/>
     </row>
@@ -956,7 +959,7 @@
         <v>43857</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" s="22"/>
     </row>
@@ -965,10 +968,10 @@
         <v>43859</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="40" t="s">
-        <v>67</v>
+        <v>26</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -985,7 +988,7 @@
         <v>43864</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10" s="19"/>
     </row>
@@ -1012,7 +1015,7 @@
         <v>43871</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13" s="21"/>
     </row>
@@ -1021,7 +1024,7 @@
         <v>43873</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C14" s="22" t="s">
         <v>4</v>
@@ -1032,7 +1035,7 @@
         <v>43876</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C15" s="18"/>
     </row>
@@ -1041,10 +1044,10 @@
         <v>43878</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1052,10 +1055,10 @@
         <v>43880</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1063,7 +1066,7 @@
         <v>43883</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" s="23"/>
     </row>
@@ -1072,7 +1075,7 @@
         <v>43885</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" s="22"/>
     </row>
@@ -1081,10 +1084,10 @@
         <v>43887</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1092,10 +1095,10 @@
         <v>43891</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1103,10 +1106,10 @@
         <v>43893</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1114,10 +1117,10 @@
         <v>43895</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1125,10 +1128,10 @@
         <v>43898</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1136,7 +1139,7 @@
         <v>43900</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C25" s="24"/>
     </row>
@@ -1145,10 +1148,10 @@
         <v>43902</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1156,7 +1159,7 @@
         <v>43905</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C27" s="19"/>
     </row>
@@ -1165,10 +1168,10 @@
         <v>43907</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1176,10 +1179,10 @@
         <v>43909</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1187,10 +1190,10 @@
         <v>43912</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1198,10 +1201,10 @@
         <v>43914</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1209,10 +1212,10 @@
         <v>43916</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1220,10 +1223,10 @@
         <v>43919</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1231,10 +1234,10 @@
         <v>43921</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1242,10 +1245,10 @@
         <v>43923</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1253,10 +1256,10 @@
         <v>43926</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" s="32" t="s">
-        <v>42</v>
+        <v>30</v>
+      </c>
+      <c r="C36" s="31" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1264,7 +1267,7 @@
         <v>43928</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C37" s="24"/>
     </row>
@@ -1273,10 +1276,10 @@
         <v>43929</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1284,21 +1287,19 @@
         <v>43933</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>58</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C39" s="19"/>
     </row>
     <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="17">
         <v>43935</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1306,16 +1307,18 @@
         <v>43937</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41" s="19"/>
+        <v>30</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="20">
         <v>43940</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C42" s="22"/>
     </row>
@@ -1324,19 +1327,19 @@
         <v>43942</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C43" s="21"/>
     </row>
-    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="20">
         <v>43944</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C44" s="28" t="s">
-        <v>38</v>
+        <v>28</v>
+      </c>
+      <c r="C44" s="41" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1344,10 +1347,10 @@
         <v>43947</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C45" s="19" t="s">
         <v>32</v>
-      </c>
-      <c r="C45" s="19" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1355,55 +1358,55 @@
         <v>43949</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="29">
+      <c r="A47" s="28">
         <v>43951</v>
       </c>
-      <c r="B47" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="C47" s="31" t="s">
-        <v>61</v>
+      <c r="B47" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="30" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="33">
+      <c r="A48" s="32">
         <v>43954</v>
       </c>
-      <c r="B48" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="C48" s="34" t="s">
-        <v>26</v>
+      <c r="B48" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" s="33" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" s="35"/>
-      <c r="B49" s="36"/>
-      <c r="C49" s="37"/>
+      <c r="A49" s="34"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="36"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="13"/>
       <c r="B50" s="12" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="13"/>
-      <c r="B51" s="38" t="s">
-        <v>65</v>
+      <c r="B51" s="37" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="13"/>
       <c r="B52" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>